<commit_message>
modified income statement template excel formatting
</commit_message>
<xml_diff>
--- a/data_raw/data/financial/income_statement_template.xlsx
+++ b/data_raw/data/financial/income_statement_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nobit/Documents/Development/Databricks_CafeShop_Project/data_raw/data/financial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E68FA4-B343-E143-AEB4-50A46F8772C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B39608-6170-0448-A279-F7BC64803369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,15 +191,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,22 +530,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="1" max="1" width="12" style="4" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="5" max="5" width="15" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -531,50 +557,50 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -591,124 +617,124 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -725,208 +751,208 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+    <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+    <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+    <row r="22" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+    <row r="24" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+    <row r="26" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4" t="s">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
+    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E31" s="2">

</xml_diff>